<commit_message>
EPBDS-8889 project deployment failed, if Spreadsheet contains a cell name that consist only with *
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/deployment2/simple2/module1.xlsx
+++ b/ITEST/itest.WebService/openl-repository/deployment2/simple2/module1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\deployment2\simple2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F5F499-D76D-4B71-BE59-780744EDB082}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31E71B7-CCFB-42E7-A661-8660BEE41133}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1620" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="33">
   <si>
     <t>Steps</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>moreValues*</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult sprWithEmptyRow(Integer myVar)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult sprWithEmptyColumn(Integer myVar)</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -169,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -542,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:F80"/>
+  <dimension ref="B5:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,11 +565,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
@@ -626,11 +636,11 @@
       <c r="E17" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
@@ -682,11 +692,11 @@
       <c r="D25" s="2"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
@@ -733,10 +743,10 @@
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="15"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -808,10 +818,10 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="24"/>
+      <c r="C58" s="25"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="17" t="s">
@@ -830,11 +840,11 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="20" t="s">
@@ -881,11 +891,11 @@
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="20" t="s">
@@ -956,8 +966,80 @@
       </c>
       <c r="D80" s="23"/>
     </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" s="25"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B89:D89"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B20:D20"/>

</xml_diff>